<commit_message>
correção de varias coisas fodas
</commit_message>
<xml_diff>
--- a/modelos_amfer.xlsx
+++ b/modelos_amfer.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fonte nobreak 24v/20a amfer telecom</t>
+          <t>fonte nobreak 12v-10a fx250 metalica amfer cor preto</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -498,14 +498,14 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>596.4299999999999</v>
+        <v>406.6</v>
       </c>
       <c r="G2" t="n">
-        <v>596.4299999999999</v>
+        <v>406.6</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FONTE NOBREAK FX500 24v/20a</t>
+          <t>FONTE NOBREAK FX250 12V/10A</t>
         </is>
       </c>
     </row>

</xml_diff>